<commit_message>
added results examen and new homeworks
</commit_message>
<xml_diff>
--- a/Экзамен/Экзамен.xlsx
+++ b/Экзамен/Экзамен.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="18195" windowHeight="13110"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="18195" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Экзамен" sheetId="1" r:id="rId1"/>
@@ -489,7 +489,7 @@
   <dimension ref="C2:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,10 +561,21 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>4</v>
+      </c>
       <c r="H5" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I5" s="1">
         <f>Домашки!D10</f>
@@ -572,7 +583,7 @@
       </c>
       <c r="J5" s="1">
         <f t="shared" si="1"/>
-        <v>4.859375</v>
+        <v>9.859375</v>
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.25">
@@ -608,9 +619,21 @@
       <c r="C7" t="s">
         <v>10</v>
       </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I7" s="1">
         <f>Домашки!D12</f>
@@ -618,7 +641,7 @@
       </c>
       <c r="J7" s="1">
         <f t="shared" si="1"/>
-        <v>0.859375</v>
+        <v>3.359375</v>
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">

</xml_diff>